<commit_message>
default\ directory updated: template settings yml files eliminated (validation and templates generation now are provided by the code.
</commit_message>
<xml_diff>
--- a/default/template_model_settings.xlsx
+++ b/default/template_model_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFDE408-F7AA-4703-A877-464C25B01CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC1F1E0-2272-46C6-B9C1-C8820B51D24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32810" yWindow="3030" windowWidth="29820" windowHeight="13880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="structure_sets" sheetId="1" r:id="rId1"/>
@@ -27,75 +27,153 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>set_key</t>
   </si>
   <si>
-    <t>symbol</t>
-  </si>
-  <si>
-    <t>table_name</t>
-  </si>
-  <si>
     <t>split_problem</t>
   </si>
   <si>
     <t>copy_from</t>
   </si>
   <si>
-    <t>a_Names, TYPE</t>
-  </si>
-  <si>
-    <t>a_Agg, TYPE</t>
-  </si>
-  <si>
     <t>set_key_name</t>
   </si>
   <si>
-    <t>set_symbol</t>
-  </si>
-  <si>
-    <t>set_table_name</t>
-  </si>
-  <si>
     <t>TRUE/FALSE</t>
   </si>
   <si>
     <t>another_set_key</t>
   </si>
   <si>
-    <t>filter_key_0: {header: [header_0, TEXT], filter_values: [val1, val2]}, filter_key_1: {header: [header_1, TEXT], filter_values: [val1, val2]}</t>
-  </si>
-  <si>
-    <t>table_structure_name</t>
-  </si>
-  <si>
-    <t>table_structure_aggregation</t>
-  </si>
-  <si>
-    <t>table_structure_filters</t>
-  </si>
-  <si>
     <t>table_key</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
+    <t>coordinates</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>cols</t>
+  </si>
+  <si>
+    <t>intra</t>
+  </si>
+  <si>
+    <t>make coefficients, physical</t>
+  </si>
+  <si>
+    <t>exogenous</t>
+  </si>
+  <si>
+    <t>sectors, products</t>
+  </si>
+  <si>
+    <t>sectors {domain: domestic}</t>
+  </si>
+  <si>
+    <t>products {physical: True}</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>v_yy</t>
+  </si>
+  <si>
+    <t>sectors {domain: domestic, dispatch: yearly}</t>
+  </si>
+  <si>
+    <t>products {physical: True, dispatch: yearly}</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>final demand by product, physical</t>
+  </si>
+  <si>
+    <t>endogenous</t>
+  </si>
+  <si>
+    <t>products, technologies, years</t>
+  </si>
+  <si>
+    <t>technologies {type_physical: final}</t>
+  </si>
+  <si>
+    <t>Q_y</t>
+  </si>
+  <si>
+    <t>total demand by technology by year</t>
+  </si>
+  <si>
+    <t>0: endogenous; 1: exogenous</t>
+  </si>
+  <si>
+    <t>products, years</t>
+  </si>
+  <si>
+    <t>E_y</t>
+  </si>
+  <si>
+    <t>products {physical: True, time_resolution: year}</t>
+  </si>
+  <si>
+    <t>years {model}</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>problem_key</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>expressions</t>
+  </si>
+  <si>
+    <t>Minimize(E)</t>
+  </si>
+  <si>
+    <t>var_1 - var_2 == 0</t>
+  </si>
+  <si>
+    <t>var_3 &gt;= 0</t>
+  </si>
+  <si>
+    <t>var_4 == 2</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>filters</t>
+  </si>
+  <si>
+    <t>filter_key_1: [val1, val2]</t>
+  </si>
+  <si>
+    <t>filter_key_0: [val1, val2]</t>
+  </si>
+  <si>
     <t>integer</t>
-  </si>
-  <si>
-    <t>coordinates</t>
-  </si>
-  <si>
-    <t>var_key</t>
-  </si>
-  <si>
-    <t>value</t>
   </si>
 </sst>
 </file>
@@ -131,13 +209,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -151,17 +236,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0">
+  <autoFilter ref="A1:E3" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B25B1879-C5E9-4EB5-B028-F8512D272279}" name="set_key"/>
-    <tableColumn id="2" xr3:uid="{CFB4F1D7-CFFC-4FE1-B14F-5C7A2795C822}" name="symbol"/>
-    <tableColumn id="3" xr3:uid="{A817388D-0FEC-4E55-A559-5E198E460C97}" name="table_name"/>
+    <tableColumn id="9" xr3:uid="{DF8CC285-45E4-43D5-B8D8-803C745D6940}" name="description"/>
     <tableColumn id="4" xr3:uid="{A3D9FB3A-774D-46EA-8E98-EFD15E392CBD}" name="split_problem"/>
     <tableColumn id="5" xr3:uid="{4DE4C0F6-8358-4391-8A54-2B4946D8B3C0}" name="copy_from"/>
-    <tableColumn id="6" xr3:uid="{1413FF9F-D2C6-4509-9E0C-146348636048}" name="table_structure_name"/>
-    <tableColumn id="7" xr3:uid="{10C048EB-6E88-4CCF-9B39-D7B0C6624180}" name="table_structure_aggregation"/>
-    <tableColumn id="8" xr3:uid="{AD5E32F7-2499-45CB-8B2A-F64E57F8E7E0}" name="table_structure_filters"/>
+    <tableColumn id="8" xr3:uid="{AD5E32F7-2499-45CB-8B2A-F64E57F8E7E0}" name="filters"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB6E5FDC-ADDB-4F17-8178-C8D1F44ADCB4}" name="Table3" displayName="Table3" ref="A1:J6" totalsRowShown="0">
+  <autoFilter ref="A1:J6" xr:uid="{DB6E5FDC-ADDB-4F17-8178-C8D1F44ADCB4}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{5A6F1C1B-5562-46B4-BC85-F746FD6D1DBE}" name="table_key"/>
+    <tableColumn id="2" xr3:uid="{E384D175-7DA2-49C7-B3FC-49DBCD470E65}" name="description"/>
+    <tableColumn id="3" xr3:uid="{C6B3D967-EA77-4A04-9D11-46C4D49CF8F6}" name="type"/>
+    <tableColumn id="13" xr3:uid="{83A8BC4B-206B-4838-8465-DA00D6AF4934}" name="integer"/>
+    <tableColumn id="4" xr3:uid="{42C7BA45-FFAE-469A-B3C2-CE76EBDED815}" name="coordinates"/>
+    <tableColumn id="5" xr3:uid="{B5D8F399-CD45-4E77-BCC7-A887EAB78252}" name="variable"/>
+    <tableColumn id="6" xr3:uid="{85ABF431-F246-4294-A409-A0264A2F184C}" name="value"/>
+    <tableColumn id="7" xr3:uid="{FEAB5FE3-58DE-4670-862E-052063177A74}" name="rows"/>
+    <tableColumn id="8" xr3:uid="{008091F5-6641-4780-81F5-35FCB69020DE}" name="cols"/>
+    <tableColumn id="9" xr3:uid="{BA148EC5-044E-42E5-9DAC-375472F19E25}" name="intra"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}" name="Table4" displayName="Table4" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{339B6BC6-DC77-44F3-BC7D-5887B7C1C68A}" name="problem_key" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{7D3A5DDD-E4D2-4BFD-8F61-20DAAF76C565}" name="objective"/>
+    <tableColumn id="3" xr3:uid="{F83410DB-FD97-4F82-A158-44491E25E434}" name="expressions"/>
+    <tableColumn id="4" xr3:uid="{43081833-0EE4-4FC1-955F-5D78145539E2}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -430,75 +544,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="112.1796875" customWidth="1"/>
-    <col min="9" max="10" width="10.54296875" customWidth="1"/>
+    <col min="1" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" customWidth="1"/>
+    <col min="6" max="7" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+      <c r="E3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -512,60 +615,276 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB1223C-005A-485D-B8DC-21499F0D118B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="5" max="5" width="29.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" customWidth="1"/>
+    <col min="8" max="8" width="37.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB4DB9B-67B8-45E9-9CD6-D02B1BE46AE7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update template_model_settings.xlsx, adding equations description.
</commit_message>
<xml_diff>
--- a/default/template_model_settings.xlsx
+++ b/default/template_model_settings.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\integrated\1_coupled_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC1F1E0-2272-46C6-B9C1-C8820B51D24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28AFD02-90F5-444D-A928-4FCA652F2259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32810" yWindow="3030" windowWidth="29820" windowHeight="13880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37640" yWindow="760" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="structure_sets" sheetId="1" r:id="rId1"/>
-    <sheet name="structure_variables" sheetId="2" r:id="rId2"/>
+    <sheet name="structure_variables" sheetId="4" r:id="rId2"/>
     <sheet name="problem" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>set_key</t>
   </si>
@@ -38,15 +38,6 @@
     <t>copy_from</t>
   </si>
   <si>
-    <t>set_key_name</t>
-  </si>
-  <si>
-    <t>TRUE/FALSE</t>
-  </si>
-  <si>
-    <t>another_set_key</t>
-  </si>
-  <si>
     <t>table_key</t>
   </si>
   <si>
@@ -59,87 +50,9 @@
     <t>value</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>rows</t>
-  </si>
-  <si>
-    <t>cols</t>
-  </si>
-  <si>
-    <t>intra</t>
-  </si>
-  <si>
-    <t>make coefficients, physical</t>
-  </si>
-  <si>
     <t>exogenous</t>
   </si>
   <si>
-    <t>sectors, products</t>
-  </si>
-  <si>
-    <t>sectors {domain: domestic}</t>
-  </si>
-  <si>
-    <t>products {physical: True}</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>v_yy</t>
-  </si>
-  <si>
-    <t>sectors {domain: domestic, dispatch: yearly}</t>
-  </si>
-  <si>
-    <t>products {physical: True, dispatch: yearly}</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>final demand by product, physical</t>
-  </si>
-  <si>
-    <t>endogenous</t>
-  </si>
-  <si>
-    <t>products, technologies, years</t>
-  </si>
-  <si>
-    <t>technologies {type_physical: final}</t>
-  </si>
-  <si>
-    <t>Q_y</t>
-  </si>
-  <si>
-    <t>total demand by technology by year</t>
-  </si>
-  <si>
-    <t>0: endogenous; 1: exogenous</t>
-  </si>
-  <si>
-    <t>products, years</t>
-  </si>
-  <si>
-    <t>E_y</t>
-  </si>
-  <si>
-    <t>products {physical: True, time_resolution: year}</t>
-  </si>
-  <si>
-    <t>years {model}</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>problem_key</t>
   </si>
   <si>
@@ -149,31 +62,121 @@
     <t>expressions</t>
   </si>
   <si>
-    <t>Minimize(E)</t>
-  </si>
-  <si>
-    <t>var_1 - var_2 == 0</t>
-  </si>
-  <si>
-    <t>var_3 &gt;= 0</t>
-  </si>
-  <si>
-    <t>var_4 == 2</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
     <t>filters</t>
   </si>
   <si>
-    <t>filter_key_1: [val1, val2]</t>
-  </si>
-  <si>
-    <t>filter_key_0: [val1, val2]</t>
-  </si>
-  <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>environmental transactions</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>products of the system</t>
+  </si>
+  <si>
+    <t>product_data</t>
+  </si>
+  <si>
+    <t>ancillary data</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>products supply</t>
+  </si>
+  <si>
+    <t>resources, products</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>energy use</t>
+  </si>
+  <si>
+    <t>products_data</t>
+  </si>
+  <si>
+    <t>product data</t>
+  </si>
+  <si>
+    <t>products, product_data</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>a_0</t>
+  </si>
+  <si>
+    <t>lr</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>energy availability</t>
+  </si>
+  <si>
+    <t>Maximize(c @ tran(x))</t>
+  </si>
+  <si>
+    <t>a @ tran(x) - b &lt;= 0</t>
+  </si>
+  <si>
+    <t>x &gt;= 0</t>
+  </si>
+  <si>
+    <t>a - a_0 - lr @ diag(x) == 0</t>
+  </si>
+  <si>
+    <t>variables_info</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>1: endogenous, 2: exogenous</t>
+  </si>
+  <si>
+    <t>1: exogenous, 2: endogenous</t>
+  </si>
+  <si>
+    <t>dim: cols</t>
+  </si>
+  <si>
+    <t>dim: rows, filters: {category: [profit]}</t>
+  </si>
+  <si>
+    <t>dim: rows, filters: {category: [energy_use_0]}</t>
+  </si>
+  <si>
+    <t>dim: rows, filters: {category: [learning_rate]}</t>
+  </si>
+  <si>
+    <t>category: [energy_use_0, learning_rate, profit]</t>
+  </si>
+  <si>
+    <t>maximization of total profit</t>
+  </si>
+  <si>
+    <t>energy use less than endowment</t>
+  </si>
+  <si>
+    <t>positive products supply</t>
+  </si>
+  <si>
+    <t>energy use per unit of product</t>
   </si>
 </sst>
 </file>
@@ -209,11 +212,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,13 +240,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0">
-  <autoFilter ref="A1:E3" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B25B1879-C5E9-4EB5-B028-F8512D272279}" name="set_key"/>
     <tableColumn id="9" xr3:uid="{DF8CC285-45E4-43D5-B8D8-803C745D6940}" name="description"/>
     <tableColumn id="4" xr3:uid="{A3D9FB3A-774D-46EA-8E98-EFD15E392CBD}" name="split_problem"/>
-    <tableColumn id="5" xr3:uid="{4DE4C0F6-8358-4391-8A54-2B4946D8B3C0}" name="copy_from"/>
+    <tableColumn id="2" xr3:uid="{63BC0DE3-0E2B-46D5-92FB-25DE1E0A2CA9}" name="copy_from"/>
     <tableColumn id="8" xr3:uid="{AD5E32F7-2499-45CB-8B2A-F64E57F8E7E0}" name="filters"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -250,19 +254,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DB6E5FDC-ADDB-4F17-8178-C8D1F44ADCB4}" name="Table3" displayName="Table3" ref="A1:J6" totalsRowShown="0">
-  <autoFilter ref="A1:J6" xr:uid="{DB6E5FDC-ADDB-4F17-8178-C8D1F44ADCB4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7FBD057B-B132-4379-814B-BD2BA1AFF594}" name="Table33" displayName="Table33" ref="A1:J7" totalsRowShown="0">
+  <autoFilter ref="A1:J7" xr:uid="{DB6E5FDC-ADDB-4F17-8178-C8D1F44ADCB4}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{5A6F1C1B-5562-46B4-BC85-F746FD6D1DBE}" name="table_key"/>
-    <tableColumn id="2" xr3:uid="{E384D175-7DA2-49C7-B3FC-49DBCD470E65}" name="description"/>
-    <tableColumn id="3" xr3:uid="{C6B3D967-EA77-4A04-9D11-46C4D49CF8F6}" name="type"/>
-    <tableColumn id="13" xr3:uid="{83A8BC4B-206B-4838-8465-DA00D6AF4934}" name="integer"/>
-    <tableColumn id="4" xr3:uid="{42C7BA45-FFAE-469A-B3C2-CE76EBDED815}" name="coordinates"/>
-    <tableColumn id="5" xr3:uid="{B5D8F399-CD45-4E77-BCC7-A887EAB78252}" name="variable"/>
-    <tableColumn id="6" xr3:uid="{85ABF431-F246-4294-A409-A0264A2F184C}" name="value"/>
-    <tableColumn id="7" xr3:uid="{FEAB5FE3-58DE-4670-862E-052063177A74}" name="rows"/>
-    <tableColumn id="8" xr3:uid="{008091F5-6641-4780-81F5-35FCB69020DE}" name="cols"/>
-    <tableColumn id="9" xr3:uid="{BA148EC5-044E-42E5-9DAC-375472F19E25}" name="intra"/>
+    <tableColumn id="1" xr3:uid="{3664E1C1-CDFB-4B96-B741-E3CF345A906A}" name="table_key"/>
+    <tableColumn id="2" xr3:uid="{5DB24C0C-CFD3-4FB5-B53C-BFA40764E5FC}" name="description"/>
+    <tableColumn id="3" xr3:uid="{2CD084FF-A0EF-4965-9069-628404776301}" name="type"/>
+    <tableColumn id="6" xr3:uid="{B7CAE23A-6C35-46F2-A86D-E8752E453E5D}" name="integer"/>
+    <tableColumn id="4" xr3:uid="{727E494E-41A0-4D77-8D19-13F369E12AD0}" name="coordinates"/>
+    <tableColumn id="5" xr3:uid="{5A4D7801-B865-4C40-AD87-418D7622F733}" name="variables_info"/>
+    <tableColumn id="10" xr3:uid="{CC0851B1-83C4-404D-8BB0-4F06479F0740}" name="value"/>
+    <tableColumn id="7" xr3:uid="{D8623746-1C30-46EA-97D5-95DE0D4F3D8A}" name="resources"/>
+    <tableColumn id="8" xr3:uid="{884F320F-DEF8-4E96-B1F4-579BB9297CB9}" name="products"/>
+    <tableColumn id="9" xr3:uid="{0DF16758-74BF-4847-8B66-F69C962A8892}" name="product_data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -275,7 +279,7 @@
     <tableColumn id="1" xr3:uid="{339B6BC6-DC77-44F3-BC7D-5887B7C1C68A}" name="problem_key" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{7D3A5DDD-E4D2-4BFD-8F61-20DAAF76C565}" name="objective"/>
     <tableColumn id="3" xr3:uid="{F83410DB-FD97-4F82-A158-44491E25E434}" name="expressions"/>
-    <tableColumn id="4" xr3:uid="{43081833-0EE4-4FC1-955F-5D78145539E2}" name="notes"/>
+    <tableColumn id="4" xr3:uid="{9BA42D33-7C36-4CDA-8AAE-32BCE0C105B1}" name="description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -544,18 +548,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="32.54296875" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+    <col min="3" max="4" width="15.08984375" customWidth="1"/>
+    <col min="5" max="5" width="51.6328125" customWidth="1"/>
     <col min="6" max="7" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -564,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -573,40 +577,43 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -614,202 +621,183 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB1223C-005A-485D-B8DC-21499F0D118B}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F872E8C-C62E-4F3F-A20F-41906D0144C1}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="29.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" customWidth="1"/>
-    <col min="8" max="8" width="37.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.36328125" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" customWidth="1"/>
+    <col min="10" max="10" width="40.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="b">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="b">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="b">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="b">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="b">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -824,29 +812,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB4DB9B-67B8-45E9-9CD6-D02B1BE46AE7}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" customWidth="1"/>
+    <col min="2" max="2" width="24.08984375" customWidth="1"/>
+    <col min="3" max="3" width="23.90625" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -854,7 +843,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -862,7 +854,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -870,7 +865,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -878,7 +876,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>